<commit_message>
Actualización Task y Schedule Team
Formatos Task y Schedule de Equipo
</commit_message>
<xml_diff>
--- a/documentos/ciclo1/TASK_TEAM.xlsx
+++ b/documentos/ciclo1/TASK_TEAM.xlsx
@@ -553,6 +553,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -562,6 +571,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -569,30 +593,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,16 +923,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -941,9 +941,9 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
@@ -957,35 +957,35 @@
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="35">
-        <v>1</v>
-      </c>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="F5" s="33">
+        <v>1</v>
+      </c>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -1020,171 +1020,171 @@
       <c r="S7" s="26"/>
     </row>
     <row r="8" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="27" t="s">
+      <c r="M8" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="27" t="s">
+      <c r="N8" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="27" t="s">
+      <c r="O8" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="P8" s="27" t="s">
+      <c r="P8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="Q8" s="27" t="s">
+      <c r="Q8" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="R8" s="27" t="s">
+      <c r="R8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="27" t="s">
+      <c r="S8" s="30" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
     </row>
     <row r="13" spans="1:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="27" t="s">
         <v>74</v>
       </c>
       <c r="B14" s="4"/>
@@ -1228,11 +1228,11 @@
       </c>
       <c r="O14" s="21">
         <f>ROUND(J14/J49*100,1)</f>
-        <v>6.4</v>
+        <v>6.7</v>
       </c>
       <c r="P14" s="17">
         <f>O14</f>
-        <v>6.4</v>
+        <v>6.7</v>
       </c>
       <c r="Q14" s="21">
         <v>9</v>
@@ -1246,7 +1246,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="9"/>
       <c r="C15" s="5" t="s">
         <v>32</v>
@@ -1288,11 +1288,11 @@
       </c>
       <c r="O15" s="21">
         <f>ROUND(J15/J49*100,1)</f>
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="P15" s="21">
         <f>SUM(O15+P14)</f>
-        <v>9.6000000000000014</v>
+        <v>10</v>
       </c>
       <c r="Q15" s="21">
         <v>6</v>
@@ -1306,7 +1306,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="9"/>
       <c r="C16" s="5" t="s">
         <v>33</v>
@@ -1315,27 +1315,27 @@
         <v>5</v>
       </c>
       <c r="E16" s="19">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F16" s="19">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="G16" s="19">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H16" s="19">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I16" s="18">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J16" s="21">
         <f t="shared" si="0"/>
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="K16" s="21">
         <f>J16+K15</f>
-        <v>16.25</v>
+        <v>17.5</v>
       </c>
       <c r="L16" s="21" t="s">
         <v>72</v>
@@ -1348,11 +1348,11 @@
       </c>
       <c r="O16" s="21">
         <f>ROUND(J16/J49*100,1)</f>
-        <v>0.8</v>
+        <v>1.7</v>
       </c>
       <c r="P16" s="21">
         <f>SUM(O16+P15)</f>
-        <v>10.400000000000002</v>
+        <v>11.7</v>
       </c>
       <c r="Q16" s="21">
         <v>1</v>
@@ -1366,7 +1366,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="27" t="s">
         <v>65</v>
       </c>
       <c r="B17" s="9"/>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="K17" s="21">
         <f t="shared" ref="K17:K48" si="2">J17+K16</f>
-        <v>21.25</v>
+        <v>22.5</v>
       </c>
       <c r="L17" s="21" t="s">
         <v>72</v>
@@ -1410,11 +1410,11 @@
       </c>
       <c r="O17" s="21">
         <f>ROUND(J17/J49*100,1)</f>
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="P17" s="21">
         <f t="shared" ref="P17:P48" si="3">SUM(O17+P16)</f>
-        <v>13.600000000000001</v>
+        <v>15</v>
       </c>
       <c r="Q17" s="21">
         <v>7</v>
@@ -1428,7 +1428,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="9"/>
       <c r="C18" s="5" t="s">
         <v>35</v>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="K18" s="21">
         <f t="shared" si="2"/>
-        <v>26.75</v>
+        <v>28</v>
       </c>
       <c r="L18" s="21" t="s">
         <v>72</v>
@@ -1470,11 +1470,11 @@
       </c>
       <c r="O18" s="21">
         <f>ROUND(J18/J49*100,1)</f>
-        <v>3.5</v>
+        <v>3.7</v>
       </c>
       <c r="P18" s="21">
         <f t="shared" si="3"/>
-        <v>17.100000000000001</v>
+        <v>18.7</v>
       </c>
       <c r="Q18" s="21">
         <v>4</v>
@@ -1488,7 +1488,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="9"/>
       <c r="C19" s="5" t="s">
         <v>75</v>
@@ -1506,18 +1506,18 @@
         <v>0</v>
       </c>
       <c r="H19" s="19">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="I19" s="23">
         <v>0</v>
       </c>
       <c r="J19" s="21">
         <f t="shared" ref="J19" si="4">SUM(E19:I19)</f>
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="K19" s="21">
         <f t="shared" ref="K19" si="5">J19+K18</f>
-        <v>27.55</v>
+        <v>28.7</v>
       </c>
       <c r="L19" s="21" t="s">
         <v>72</v>
@@ -1534,14 +1534,14 @@
       </c>
       <c r="P19" s="21">
         <f t="shared" ref="P19" si="6">SUM(O19+P18)</f>
-        <v>17.600000000000001</v>
+        <v>19.2</v>
       </c>
       <c r="Q19" s="21"/>
       <c r="R19" s="21"/>
       <c r="S19" s="21"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="27" t="s">
         <v>66</v>
       </c>
       <c r="B20" s="9"/>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="K20" s="21">
         <f>J20+K19</f>
-        <v>30.55</v>
+        <v>31.7</v>
       </c>
       <c r="L20" s="21" t="s">
         <v>72</v>
@@ -1585,18 +1585,18 @@
       </c>
       <c r="O20" s="21">
         <f>ROUND(J20/J49*100,1)</f>
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="P20" s="21">
         <f>SUM(O20+P19)</f>
-        <v>19.5</v>
+        <v>21.2</v>
       </c>
       <c r="Q20" s="21"/>
       <c r="R20" s="21"/>
       <c r="S20" s="21"/>
     </row>
     <row r="21" spans="1:19" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="9"/>
       <c r="C21" s="5" t="s">
         <v>37</v>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="K21" s="21">
         <f t="shared" si="2"/>
-        <v>32.049999999999997</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="L21" s="21" t="s">
         <v>72</v>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="P21" s="21">
         <f t="shared" si="3"/>
-        <v>20.5</v>
+        <v>22.2</v>
       </c>
       <c r="Q21" s="21">
         <v>2</v>
@@ -1651,7 +1651,7 @@
       <c r="S21" s="21"/>
     </row>
     <row r="22" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="9"/>
       <c r="C22" s="5" t="s">
         <v>38</v>
@@ -1660,27 +1660,27 @@
         <v>5</v>
       </c>
       <c r="E22" s="19">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="F22" s="19">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G22" s="19">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H22" s="19">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="I22" s="18">
         <v>1.5</v>
       </c>
       <c r="J22" s="21">
         <f t="shared" si="0"/>
-        <v>2.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K22" s="21">
         <f t="shared" si="2"/>
-        <v>34.75</v>
+        <v>35.5</v>
       </c>
       <c r="L22" s="21" t="s">
         <v>72</v>
@@ -1693,18 +1693,18 @@
       </c>
       <c r="O22" s="21">
         <f>ROUND(J22/J49*100,1)</f>
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="P22" s="21">
         <f t="shared" si="3"/>
-        <v>22.2</v>
+        <v>23.7</v>
       </c>
       <c r="Q22" s="21"/>
       <c r="R22" s="8"/>
       <c r="S22" s="21"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="9"/>
       <c r="C23" s="5" t="s">
         <v>39</v>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="K23" s="21">
         <f>J23+K22</f>
-        <v>37.75</v>
+        <v>38.5</v>
       </c>
       <c r="L23" s="21" t="s">
         <v>72</v>
@@ -1746,18 +1746,18 @@
       </c>
       <c r="O23" s="21">
         <f>ROUND(J23/J49*100,1)</f>
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="P23" s="21">
         <f>SUM(O23+P22)</f>
-        <v>24.099999999999998</v>
+        <v>25.7</v>
       </c>
       <c r="Q23" s="21"/>
       <c r="R23" s="8"/>
       <c r="S23" s="21"/>
     </row>
     <row r="24" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="40"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="9"/>
       <c r="C24" s="5" t="s">
         <v>40</v>
@@ -1766,27 +1766,27 @@
         <v>5</v>
       </c>
       <c r="E24" s="19">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="F24" s="19">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G24" s="19">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H24" s="19">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I24" s="18">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="J24" s="21">
         <f t="shared" si="0"/>
-        <v>2.6999999999999997</v>
+        <v>1.8</v>
       </c>
       <c r="K24" s="21">
         <f t="shared" si="2"/>
-        <v>40.450000000000003</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="L24" s="21" t="s">
         <v>72</v>
@@ -1799,18 +1799,18 @@
       </c>
       <c r="O24" s="21">
         <f>ROUND(J24/J49*100,1)</f>
-        <v>1.7</v>
+        <v>1.2</v>
       </c>
       <c r="P24" s="21">
         <f t="shared" si="3"/>
-        <v>25.799999999999997</v>
+        <v>26.9</v>
       </c>
       <c r="Q24" s="21"/>
       <c r="R24" s="8"/>
       <c r="S24" s="21"/>
     </row>
     <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="40"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="9"/>
       <c r="C25" s="5" t="s">
         <v>41</v>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="K25" s="21">
         <f t="shared" si="2"/>
-        <v>43.25</v>
+        <v>43.099999999999994</v>
       </c>
       <c r="L25" s="21" t="s">
         <v>72</v>
@@ -1852,18 +1852,18 @@
       </c>
       <c r="O25" s="21">
         <f>ROUND(J25/J49*100,1)</f>
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="P25" s="21">
         <f t="shared" si="3"/>
-        <v>27.599999999999998</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="Q25" s="21"/>
       <c r="R25" s="8"/>
       <c r="S25" s="21"/>
     </row>
     <row r="26" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="39"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="9"/>
       <c r="C26" s="5" t="s">
         <v>42</v>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="K26" s="21">
         <f t="shared" si="2"/>
-        <v>58.25</v>
+        <v>58.099999999999994</v>
       </c>
       <c r="L26" s="21" t="s">
         <v>72</v>
@@ -1903,18 +1903,18 @@
       <c r="N26" s="8"/>
       <c r="O26" s="21">
         <f>ROUND(J26/J49*100,1)</f>
-        <v>9.6999999999999993</v>
+        <v>10</v>
       </c>
       <c r="P26" s="21">
         <f t="shared" si="3"/>
-        <v>37.299999999999997</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="Q26" s="21"/>
       <c r="R26" s="8"/>
       <c r="S26" s="21"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="28" t="s">
         <v>67</v>
       </c>
       <c r="B27" s="9"/>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="K27" s="21">
         <f>J27+K26</f>
-        <v>64.25</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="L27" s="21" t="s">
         <v>72</v>
@@ -1956,18 +1956,18 @@
       <c r="N27" s="8"/>
       <c r="O27" s="21">
         <f>ROUND(J27/J49*100,1)</f>
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="P27" s="21">
         <f>SUM(O27+P26)</f>
-        <v>41.199999999999996</v>
+        <v>42.8</v>
       </c>
       <c r="Q27" s="21"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="40"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="9"/>
       <c r="C28" s="5" t="s">
         <v>44</v>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="K28" s="21">
         <f t="shared" si="2"/>
-        <v>67.25</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="L28" s="21" t="s">
         <v>72</v>
@@ -2007,18 +2007,18 @@
       <c r="N28" s="8"/>
       <c r="O28" s="21">
         <f>ROUND(J28/J49*100,1)</f>
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="P28" s="21">
         <f t="shared" si="3"/>
-        <v>43.099999999999994</v>
+        <v>44.8</v>
       </c>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="40"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="9"/>
       <c r="C29" s="5" t="s">
         <v>45</v>
@@ -2039,15 +2039,15 @@
         <v>2</v>
       </c>
       <c r="I29" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" s="21">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K29" s="21">
         <f>J29+K28</f>
-        <v>71.25</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="L29" s="21" t="s">
         <v>72</v>
@@ -2058,24 +2058,24 @@
       <c r="N29" s="8"/>
       <c r="O29" s="21">
         <f>ROUND(J29/J49*100,1)</f>
-        <v>2.6</v>
+        <v>2</v>
       </c>
       <c r="P29" s="21">
         <f>SUM(O29+P28)</f>
-        <v>45.699999999999996</v>
+        <v>46.8</v>
       </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="9"/>
       <c r="C30" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D30" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="19">
         <v>0</v>
@@ -2087,10 +2087,10 @@
         <v>0</v>
       </c>
       <c r="H30" s="19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I30" s="18">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="J30" s="21">
         <f t="shared" si="0"/>
@@ -2098,7 +2098,7 @@
       </c>
       <c r="K30" s="21">
         <f t="shared" si="2"/>
-        <v>73.25</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="L30" s="21" t="s">
         <v>72</v>
@@ -2113,14 +2113,14 @@
       </c>
       <c r="P30" s="21">
         <f t="shared" si="3"/>
-        <v>46.999999999999993</v>
+        <v>48.099999999999994</v>
       </c>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B31" s="9"/>
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="19">
         <v>1</v>
@@ -2147,11 +2147,11 @@
       </c>
       <c r="J31" s="21">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K31" s="21">
         <f>J31+K30</f>
-        <v>76.25</v>
+        <v>74.099999999999994</v>
       </c>
       <c r="L31" s="21" t="s">
         <v>72</v>
@@ -2162,18 +2162,18 @@
       <c r="N31" s="8"/>
       <c r="O31" s="21">
         <f>ROUND(J31/J49*100,1)</f>
-        <v>1.9</v>
+        <v>1.3</v>
       </c>
       <c r="P31" s="21">
         <f>SUM(O31+P30)</f>
-        <v>48.899999999999991</v>
+        <v>49.399999999999991</v>
       </c>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="40"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="9"/>
       <c r="C32" s="5" t="s">
         <v>48</v>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="K32" s="21">
         <f t="shared" si="2"/>
-        <v>79.25</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="L32" s="21" t="s">
         <v>72</v>
@@ -2213,18 +2213,18 @@
       <c r="N32" s="8"/>
       <c r="O32" s="21">
         <f>ROUND(J32/J49*100,1)</f>
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="P32" s="21">
         <f t="shared" si="3"/>
-        <v>50.79999999999999</v>
+        <v>51.399999999999991</v>
       </c>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
     </row>
     <row r="33" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="40"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="9"/>
       <c r="C33" s="5" t="s">
         <v>49</v>
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H33" s="19">
         <v>0</v>
@@ -2249,11 +2249,11 @@
       </c>
       <c r="J33" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K33" s="21">
         <f t="shared" si="2"/>
-        <v>80.25</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="L33" s="21" t="s">
         <v>72</v>
@@ -2264,18 +2264,18 @@
       <c r="N33" s="8"/>
       <c r="O33" s="21">
         <f>ROUND(J33/J49*100,1)</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="P33" s="21">
         <f t="shared" si="3"/>
-        <v>51.399999999999991</v>
+        <v>52.399999999999991</v>
       </c>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="40"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="9"/>
       <c r="C34" s="5" t="s">
         <v>50</v>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="K34" s="21">
         <f t="shared" si="2"/>
-        <v>83.25</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="L34" s="21" t="s">
         <v>72</v>
@@ -2315,18 +2315,18 @@
       <c r="N34" s="8"/>
       <c r="O34" s="21">
         <f>ROUND(J34/J49*100,1)</f>
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="P34" s="21">
         <f t="shared" si="3"/>
-        <v>53.29999999999999</v>
+        <v>54.399999999999991</v>
       </c>
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="39"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="9"/>
       <c r="C35" s="5" t="s">
         <v>51</v>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="K35" s="21">
         <f t="shared" si="2"/>
-        <v>88.75</v>
+        <v>87.1</v>
       </c>
       <c r="L35" s="21" t="s">
         <v>72</v>
@@ -2366,18 +2366,18 @@
       <c r="N35" s="8"/>
       <c r="O35" s="21">
         <f>ROUND(J35/J49*100,1)</f>
-        <v>3.5</v>
+        <v>3.7</v>
       </c>
       <c r="P35" s="21">
         <f t="shared" si="3"/>
-        <v>56.79999999999999</v>
+        <v>58.099999999999994</v>
       </c>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="27" t="s">
         <v>69</v>
       </c>
       <c r="B36" s="9"/>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="K36" s="21">
         <f t="shared" si="2"/>
-        <v>91.75</v>
+        <v>90.1</v>
       </c>
       <c r="L36" s="21" t="s">
         <v>72</v>
@@ -2419,18 +2419,18 @@
       <c r="N36" s="8"/>
       <c r="O36" s="21">
         <f>ROUND(J36/J49*100,1)</f>
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="P36" s="21">
         <f t="shared" si="3"/>
-        <v>58.699999999999989</v>
+        <v>60.099999999999994</v>
       </c>
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="40"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="9"/>
       <c r="C37" s="5" t="s">
         <v>53</v>
@@ -2439,7 +2439,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F37" s="19">
         <v>0</v>
@@ -2455,11 +2455,11 @@
       </c>
       <c r="J37" s="21">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="K37" s="21">
         <f t="shared" si="2"/>
-        <v>94.25</v>
+        <v>92.1</v>
       </c>
       <c r="L37" s="21" t="s">
         <v>72</v>
@@ -2470,18 +2470,18 @@
       <c r="N37" s="8"/>
       <c r="O37" s="21">
         <f>ROUND(J37/J49*100,1)</f>
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="P37" s="21">
         <f t="shared" si="3"/>
-        <v>60.29999999999999</v>
+        <v>61.399999999999991</v>
       </c>
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="40"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="9"/>
       <c r="C38" s="5" t="s">
         <v>54</v>
@@ -2510,25 +2510,25 @@
       </c>
       <c r="K38" s="21">
         <f t="shared" si="2"/>
-        <v>95.25</v>
+        <v>93.1</v>
       </c>
       <c r="L38" s="21"/>
       <c r="M38" s="21"/>
       <c r="N38" s="8"/>
       <c r="O38" s="21">
         <f>ROUND(J38/J49*100,1)</f>
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="P38" s="21">
         <f t="shared" si="3"/>
-        <v>60.899999999999991</v>
+        <v>62.099999999999994</v>
       </c>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="40"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="9"/>
       <c r="C39" s="5" t="s">
         <v>55</v>
@@ -2543,10 +2543,10 @@
         <v>0</v>
       </c>
       <c r="G39" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="18">
         <v>1</v>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="K39" s="21">
         <f t="shared" si="2"/>
-        <v>97.25</v>
+        <v>95.1</v>
       </c>
       <c r="L39" s="21" t="s">
         <v>72</v>
@@ -2570,14 +2570,14 @@
       </c>
       <c r="P39" s="21">
         <f t="shared" si="3"/>
-        <v>62.199999999999989</v>
+        <v>63.399999999999991</v>
       </c>
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="40"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="9"/>
       <c r="C40" s="5" t="s">
         <v>56</v>
@@ -2595,18 +2595,18 @@
         <v>0.5</v>
       </c>
       <c r="H40" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" s="18">
         <v>1</v>
       </c>
       <c r="J40" s="21">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="K40" s="21">
         <f t="shared" si="2"/>
-        <v>99.75</v>
+        <v>96.6</v>
       </c>
       <c r="L40" s="21" t="s">
         <v>72</v>
@@ -2617,18 +2617,18 @@
       <c r="N40" s="8"/>
       <c r="O40" s="21">
         <f>ROUND(J40/J49*100,1)</f>
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="P40" s="21">
         <f t="shared" si="3"/>
-        <v>63.79999999999999</v>
+        <v>64.399999999999991</v>
       </c>
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
     <row r="41" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="40"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="9"/>
       <c r="C41" s="5" t="s">
         <v>57</v>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="K41" s="21">
         <f t="shared" si="2"/>
-        <v>124.75</v>
+        <v>121.6</v>
       </c>
       <c r="L41" s="21" t="s">
         <v>73</v>
@@ -2668,18 +2668,18 @@
       <c r="N41" s="8"/>
       <c r="O41" s="21">
         <f>ROUND(J41/J49*100,1)</f>
-        <v>16.100000000000001</v>
+        <v>16.7</v>
       </c>
       <c r="P41" s="21">
         <f t="shared" si="3"/>
-        <v>79.899999999999991</v>
+        <v>81.099999999999994</v>
       </c>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="40"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="9"/>
       <c r="C42" s="5" t="s">
         <v>58</v>
@@ -2688,7 +2688,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="19">
         <v>1</v>
@@ -2704,29 +2704,29 @@
       </c>
       <c r="J42" s="21">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K42" s="21">
         <f t="shared" si="2"/>
-        <v>127.75</v>
+        <v>123.6</v>
       </c>
       <c r="L42" s="21"/>
       <c r="M42" s="21"/>
       <c r="N42" s="8"/>
       <c r="O42" s="21">
         <f>ROUND(J42/J49*100,1)</f>
-        <v>1.9</v>
+        <v>1.3</v>
       </c>
       <c r="P42" s="21">
         <f t="shared" si="3"/>
-        <v>81.8</v>
+        <v>82.399999999999991</v>
       </c>
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
       <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="39"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="9"/>
       <c r="C43" s="5" t="s">
         <v>59</v>
@@ -2738,24 +2738,24 @@
         <v>0</v>
       </c>
       <c r="F43" s="19">
+        <v>0</v>
+      </c>
+      <c r="G43" s="19">
+        <v>0</v>
+      </c>
+      <c r="H43" s="19">
         <v>0.5</v>
-      </c>
-      <c r="G43" s="19">
-        <v>0</v>
-      </c>
-      <c r="H43" s="19">
-        <v>1</v>
       </c>
       <c r="I43" s="18">
         <v>0.5</v>
       </c>
       <c r="J43" s="21">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K43" s="21">
         <f t="shared" si="2"/>
-        <v>129.75</v>
+        <v>124.6</v>
       </c>
       <c r="L43" s="21" t="s">
         <v>72</v>
@@ -2766,7 +2766,7 @@
       <c r="N43" s="8"/>
       <c r="O43" s="21">
         <f>ROUND(J43/J49*100,1)</f>
-        <v>1.3</v>
+        <v>0.7</v>
       </c>
       <c r="P43" s="21">
         <f t="shared" si="3"/>
@@ -2777,7 +2777,7 @@
       <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="27" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="9"/>
@@ -2808,7 +2808,7 @@
       </c>
       <c r="K44" s="21">
         <f t="shared" si="2"/>
-        <v>134.75</v>
+        <v>129.6</v>
       </c>
       <c r="L44" s="21" t="s">
         <v>72</v>
@@ -2819,18 +2819,18 @@
       <c r="N44" s="8"/>
       <c r="O44" s="21">
         <f>ROUND(J44/J49*100,1)</f>
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="P44" s="21">
         <f t="shared" si="3"/>
-        <v>86.3</v>
+        <v>86.399999999999991</v>
       </c>
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="40"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="9"/>
       <c r="C45" s="5" t="s">
         <v>61</v>
@@ -2859,25 +2859,25 @@
       </c>
       <c r="K45" s="21">
         <f t="shared" si="2"/>
-        <v>137.75</v>
+        <v>132.6</v>
       </c>
       <c r="L45" s="21"/>
       <c r="M45" s="21"/>
       <c r="N45" s="8"/>
       <c r="O45" s="21">
         <f>ROUND(J45/J49*100,1)</f>
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="P45" s="21">
         <f t="shared" si="3"/>
-        <v>88.2</v>
+        <v>88.399999999999991</v>
       </c>
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="39"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="9"/>
       <c r="C46" s="5" t="s">
         <v>62</v>
@@ -2906,7 +2906,7 @@
       </c>
       <c r="K46" s="21">
         <f t="shared" si="2"/>
-        <v>142.75</v>
+        <v>137.6</v>
       </c>
       <c r="L46" s="21" t="s">
         <v>72</v>
@@ -2917,18 +2917,18 @@
       <c r="N46" s="8"/>
       <c r="O46" s="21">
         <f>ROUND(J46/J49*100,1)</f>
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="P46" s="21">
         <f t="shared" si="3"/>
-        <v>91.4</v>
+        <v>91.699999999999989</v>
       </c>
       <c r="Q46" s="8"/>
       <c r="R46" s="8"/>
       <c r="S46" s="8"/>
     </row>
     <row r="47" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="27" t="s">
         <v>71</v>
       </c>
       <c r="B47" s="9"/>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="K47" s="21">
         <f t="shared" si="2"/>
-        <v>147.75</v>
+        <v>142.6</v>
       </c>
       <c r="L47" s="21" t="s">
         <v>72</v>
@@ -2970,18 +2970,18 @@
       <c r="N47" s="8"/>
       <c r="O47" s="21">
         <f>ROUND(J47/J49*100,1)</f>
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="P47" s="21">
         <f t="shared" si="3"/>
-        <v>94.600000000000009</v>
+        <v>94.999999999999986</v>
       </c>
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="39"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="10"/>
       <c r="C48" s="11" t="s">
         <v>64</v>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="K48" s="21">
         <f t="shared" si="2"/>
-        <v>155.25</v>
+        <v>150.1</v>
       </c>
       <c r="L48" s="22" t="s">
         <v>72</v>
@@ -3021,11 +3021,11 @@
       <c r="N48" s="12"/>
       <c r="O48" s="21">
         <f>ROUND(J48/J49*100,1)</f>
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="P48" s="21">
         <f t="shared" si="3"/>
-        <v>99.4</v>
+        <v>99.999999999999986</v>
       </c>
       <c r="Q48" s="8"/>
       <c r="R48" s="12"/>
@@ -3038,27 +3038,27 @@
       <c r="D49" s="14"/>
       <c r="E49" s="6">
         <f t="shared" ref="E49:J49" si="7">SUM(E14:E48)</f>
-        <v>31.35</v>
+        <v>29.9</v>
       </c>
       <c r="F49" s="6">
         <f t="shared" si="7"/>
-        <v>30.55</v>
+        <v>30.099999999999998</v>
       </c>
       <c r="G49" s="6">
         <f t="shared" si="7"/>
-        <v>31.55</v>
+        <v>30.099999999999998</v>
       </c>
       <c r="H49" s="6">
         <f t="shared" si="7"/>
-        <v>31.549999999999997</v>
+        <v>30.1</v>
       </c>
       <c r="I49" s="7">
         <f t="shared" si="7"/>
-        <v>30.25</v>
+        <v>29.9</v>
       </c>
       <c r="J49" s="21">
-        <f t="shared" si="7"/>
-        <v>155.25</v>
+        <f>SUM(J14:J48)</f>
+        <v>150.1</v>
       </c>
       <c r="K49" s="14"/>
       <c r="L49" s="13"/>
@@ -3066,7 +3066,7 @@
       <c r="N49" s="15"/>
       <c r="O49" s="21">
         <f>SUM(O14:O48)</f>
-        <v>99.4</v>
+        <v>99.999999999999986</v>
       </c>
       <c r="P49" s="15"/>
       <c r="Q49" s="8"/>
@@ -3078,28 +3078,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="P8:P13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="N8:N13"/>
-    <mergeCell ref="O8:O13"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="K8:K13"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B8:B13"/>
@@ -3116,6 +3094,28 @@
     <mergeCell ref="J8:J13"/>
     <mergeCell ref="L8:L13"/>
     <mergeCell ref="M8:M13"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="K8:K13"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="P8:P13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="N8:N13"/>
+    <mergeCell ref="O8:O13"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>